<commit_message>
Update Jan before matchday 20
</commit_message>
<xml_diff>
--- a/fantacalcio/seriea_calendar.xlsx
+++ b/fantacalcio/seriea_calendar.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\fantabeto\fantacalcio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\fantabeto\fantacalcio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD6D618-A8F5-4A2E-99F6-79AD2663AC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C4118F-60E3-4F5E-9DF1-CBA4AAAA3527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1110" windowWidth="29040" windowHeight="15720" xr2:uid="{C559B230-65AC-458C-A866-22DEA9D55CFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="418">
   <si>
     <t xml:space="preserve">1 (14/8/22)
 </t>
@@ -678,48 +678,6 @@
     <t>Spezia-Roma</t>
   </si>
   <si>
-    <t>1 (14/8/22)</t>
-  </si>
-  <si>
-    <t>2 (28/8/22)</t>
-  </si>
-  <si>
-    <t>3 (28/8/22)</t>
-  </si>
-  <si>
-    <t>4 (31/8/22)</t>
-  </si>
-  <si>
-    <t>6 (11/9/22)</t>
-  </si>
-  <si>
-    <t>8 (2/10/22)</t>
-  </si>
-  <si>
-    <t>10 (16/10/22)</t>
-  </si>
-  <si>
-    <t>11 (23/10/22)</t>
-  </si>
-  <si>
-    <t>12 (30/10/22)</t>
-  </si>
-  <si>
-    <t>13 (6/11/22)</t>
-  </si>
-  <si>
-    <t>14 (9/11/22 )</t>
-  </si>
-  <si>
-    <t>15 (13/11/22)</t>
-  </si>
-  <si>
-    <t>17 (8/1/23)</t>
-  </si>
-  <si>
-    <t>18 (15/1/23)</t>
-  </si>
-  <si>
     <t>Cremonese-Fiorentina</t>
   </si>
   <si>
@@ -738,9 +696,6 @@
     <t>Udinese-Milan</t>
   </si>
   <si>
-    <t>Torino-Monza</t>
-  </si>
-  <si>
     <t>Roma-Salernitana</t>
   </si>
   <si>
@@ -783,9 +738,6 @@
     <t>Torino-Cremonese</t>
   </si>
   <si>
-    <t>Napoli-Fiorentina</t>
-  </si>
-  <si>
     <t>Atalanta-Verona</t>
   </si>
   <si>
@@ -858,9 +810,6 @@
     <t>Atalanta-Monza</t>
   </si>
   <si>
-    <t>Empoli-Salernitana</t>
-  </si>
-  <si>
     <t>Bologna-Spezia</t>
   </si>
   <si>
@@ -939,9 +888,6 @@
     <t>Udinese-Verona</t>
   </si>
   <si>
-    <t>Roma-Inter</t>
-  </si>
-  <si>
     <t>Spezia-Lazio</t>
   </si>
   <si>
@@ -1014,9 +960,6 @@
     <t>Roma-Sampdoria</t>
   </si>
   <si>
-    <t>Cremonese-Spezia</t>
-  </si>
-  <si>
     <t>Juventus-Torino</t>
   </si>
   <si>
@@ -1143,9 +1086,6 @@
     <t>Inter-Atalanta</t>
   </si>
   <si>
-    <t>Sassuolo-Bologna</t>
-  </si>
-  <si>
     <t>Spezia-Verona</t>
   </si>
   <si>
@@ -1266,28 +1206,117 @@
     <t>Torino-Fiorentina</t>
   </si>
   <si>
-    <t>Lecce-Verona</t>
-  </si>
-  <si>
     <t>Empoli-Inter</t>
   </si>
   <si>
-    <t>Atalanta-Juventus</t>
-  </si>
-  <si>
-    <t>Milan-Lazio</t>
-  </si>
-  <si>
     <t>Sassuolo-Monza</t>
   </si>
   <si>
     <t>Napoli-Salernitana</t>
   </si>
   <si>
-    <t>Udinese-Sampdoria</t>
-  </si>
-  <si>
     <t>Roma-Spezia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 (29/1/23)
+</t>
+  </si>
+  <si>
+    <t>26 (12/3/23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 (30/4/23)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 (5/2/23)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 (19/3/23)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33 (3/5/23 )
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 (12/2/23)
+</t>
+  </si>
+  <si>
+    <t>28 (2/4/23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34 (7/5/23)
+</t>
+  </si>
+  <si>
+    <t>ATALANTA-JUVENTUS</t>
+  </si>
+  <si>
+    <t>CREMONESE-SPEZIA</t>
+  </si>
+  <si>
+    <t>EMPOLI-SALERNITANA</t>
+  </si>
+  <si>
+    <t>LECCE-VERONA</t>
+  </si>
+  <si>
+    <t>MILAN-LAZIO</t>
+  </si>
+  <si>
+    <t>NAPOLI-FIORENTINA</t>
+  </si>
+  <si>
+    <t>ROMA-INTER</t>
+  </si>
+  <si>
+    <t>SASSUOLO-BOLOGNA</t>
+  </si>
+  <si>
+    <t>TORINO-MONZA</t>
+  </si>
+  <si>
+    <t>UDINESE-SAMPDORIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 (19/2/23)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 (8/4/23)
+</t>
+  </si>
+  <si>
+    <t>35 (14/5/23)</t>
+  </si>
+  <si>
+    <t>24 (26/2/23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 (16/4/23)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36 (21/5/23)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 (5/3/23)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 (23/4/23)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37 (28/5/23)
+</t>
+  </si>
+  <si>
+    <t>38 (4/6/23)</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1402,11 +1431,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1427,6 +1501,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1735,7 +1818,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1745,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A162C09C-D7D0-4C10-B045-2A655C3577C1}">
   <dimension ref="A1:A418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="A215" sqref="A215"/>
+    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="A210" sqref="A210:A418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2794,1057 +2877,2118 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="6" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+    <row r="210" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A211" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A212" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A213" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A215" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A216" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A220" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A231" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A232" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A243" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A244" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A246" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A247" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A248" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A249" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A251" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A252" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A253" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A254" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A255" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A256" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A257" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A258" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A259" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A260" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A261" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A262" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A263" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A264" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A265" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A266" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A267" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A268" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A269" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A270" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A271" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A272" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A273" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A274" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A275" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A276" s="9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A277" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A278" s="6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+    <row r="279" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A279" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A280" s="6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A281" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+    <row r="282" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A282" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A283" s="6" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A284" s="6" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A285" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A286" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A287" s="4" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A288" s="6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A289" s="6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A290" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A291" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A292" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A293" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A294" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A295" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A296" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A297" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A298" s="5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A299" s="6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A300" s="6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A301" s="6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A302" s="6" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A303" s="6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A304" s="6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A305" s="6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A306" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A307" s="6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A308" s="6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A309" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A310" s="6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A311" s="6" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A312" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A313" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A314" s="6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A315" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A316" s="6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A317" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A318" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A319" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A320" s="5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A321" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A322" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A323" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A324" s="6" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A325" s="6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A326" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A327" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A328" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A329" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A330" s="6" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A331" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A332" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A333" s="6" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A334" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A335" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A336" s="6" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+    <row r="337" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A337" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A338" s="6" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A339" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A340" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A341" s="6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A342" s="10" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A343" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A344" s="6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A345" s="6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A346" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A347" s="6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A348" s="6" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A349" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A350" s="6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A351" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A352" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A353" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A354" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A355" s="6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A356" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A357" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A358" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A359" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A360" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A361" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A362" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A363" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A364" s="5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A365" s="6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A366" s="6" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A367" s="6" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A368" s="6" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A369" s="6" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A370" s="6" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A371" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A372" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A373" s="6" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A374" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A375" s="5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A376" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A377" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A378" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A379" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A380" s="6" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A381" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A382" s="6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A383" s="6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A384" s="6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A385" s="6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A386" s="5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A387" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A388" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A389" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A390" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A391" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A392" s="6" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A393" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A394" s="6" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A395" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A396" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A397" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A398" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A399" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A400" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A401" s="6" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
+    <row r="402" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A402" s="6" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A403" s="6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A404" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A405" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A406" s="6" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
+    <row r="407" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A407" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A408" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A409" s="6" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
+    <row r="410" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A410" s="6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A411" s="6" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A412" s="6" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A413" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A414" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A415" s="6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A416" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A417" s="6" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A265" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A318" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A325" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A333" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A339" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A346" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A349" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A355" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A358" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" t="s">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" s="6" t="s">
         <v>366</v>
-      </c>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A378" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A393" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A399" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A406" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" t="s">
-        <v>412</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E3DE5D-F672-4D6D-8316-E0AFC3F54BAF}">
+  <dimension ref="A1:A209"/>
+  <sheetViews>
+    <sheetView topLeftCell="A181" workbookViewId="0">
+      <selection sqref="A1:A209"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="6" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="6" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="6" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="6" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="6" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="6" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="6" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="6" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="10" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="6" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="6" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="6" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="6" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="6" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="6" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="6" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="6" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="6" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="6" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="6" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="6" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A203" s="6" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A209" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>